<commit_message>
fixed correct week freq
</commit_message>
<xml_diff>
--- a/Sufficient data/forecast_summary_B083NMK4BB.xlsx
+++ b/Sufficient data/forecast_summary_B083NMK4BB.xlsx
@@ -719,7 +719,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
@@ -947,7 +947,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2023-09-10</t>
+          <t>2023-10-15</t>
         </is>
       </c>
     </row>

</xml_diff>